<commit_message>
4/27/2017 * Added MAPE and Median percent error to data output and summary tables
* Added graphics to summary tables

* Fixed error in code that was not computing consumption correctly
</commit_message>
<xml_diff>
--- a/Summary Tables and Graphics.xlsx
+++ b/Summary Tables and Graphics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Site" sheetId="1" r:id="rId1"/>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>